<commit_message>
removed consent, removed extra Qs, reduced trials from 9 to 4, 2 trials for letters, 2 trials for categories
</commit_message>
<xml_diff>
--- a/condition.xlsx
+++ b/condition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canfenerci/Dropbox/My Mac (sheldonmemorylab2s-iMac.local)/Desktop/Fluency Task/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adkinsty/files/experiments/fluency-task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63961085-4ECA-4447-AB78-BE0B21FF5124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019DADD9-808F-8244-863F-00D8FEF691F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="460" windowWidth="20060" windowHeight="15200" xr2:uid="{4D1270A6-E747-4494-A784-B9E0480AD422}"/>
+    <workbookView xWindow="8020" yWindow="500" windowWidth="20060" windowHeight="15200" xr2:uid="{4D1270A6-E747-4494-A784-B9E0480AD422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Category</t>
   </si>
@@ -39,18 +39,12 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Spatial</t>
-  </si>
-  <si>
     <t>Phonemic</t>
   </si>
   <si>
     <t>Semantic</t>
   </si>
   <si>
-    <t>Words that start with F</t>
-  </si>
-  <si>
     <t>Words that start with A</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Occupations</t>
   </si>
   <si>
-    <t>Sports</t>
-  </si>
-  <si>
     <t>LET</t>
   </si>
   <si>
@@ -73,15 +64,6 @@
   </si>
   <si>
     <t>p</t>
-  </si>
-  <si>
-    <t>Things in a Restaurant</t>
-  </si>
-  <si>
-    <t>Things in a Hotel Lobby</t>
-  </si>
-  <si>
-    <t>Things in a Garage</t>
   </si>
 </sst>
 </file>
@@ -433,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1DBBE6-C4ED-4CA8-A503-B6DF6C8D1BA5}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -453,106 +435,51 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
         <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>